<commit_message>
Refactor the ESPHome atom config files.
</commit_message>
<xml_diff>
--- a/UI/Button_Mapping.xlsx
+++ b/UI/Button_Mapping.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t xml:space="preserve">Button_Device_MQTT_Prefix</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Composite_State</t>
   </si>
   <si>
-    <t xml:space="preserve">lighting/buttons/atom_01</t>
+    <t xml:space="preserve">lighting/buttons/atom-01</t>
   </si>
   <si>
     <t xml:space="preserve">a</t>
@@ -52,10 +52,10 @@
     <t xml:space="preserve">Meeting_Room</t>
   </si>
   <si>
-    <t xml:space="preserve">lighting/buttons/atom_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighting/buttons/atom_03</t>
+    <t xml:space="preserve">lighting/buttons/atom-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-03</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1a/switch/channel_10</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Basement</t>
   </si>
   <si>
-    <t xml:space="preserve">lighting/buttons/atom_04</t>
+    <t xml:space="preserve">lighting/buttons/atom-04</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1c/switch/channel_2</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Forge</t>
   </si>
   <si>
-    <t xml:space="preserve">lighting/buttons/atom_05</t>
+    <t xml:space="preserve">lighting/buttons/atom-05</t>
   </si>
   <si>
     <t xml:space="preserve">lighting/panel_1c/switch/channel_6</t>
@@ -89,6 +89,81 @@
   </si>
   <si>
     <t xml:space="preserve">Welding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighting/buttons/atom-30</t>
   </si>
 </sst>
 </file>
@@ -103,6 +178,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -265,10 +341,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,7 +413,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -375,7 +451,7 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -392,6 +468,206 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>